<commit_message>
COST Pricing model lab update
</commit_message>
<xml_diff>
--- a/Cost/Cost_Fundamentals/200_3_Pricing_Models/Code/Combined_EC2_RI_Rec.xlsx
+++ b/Cost/Cost_Fundamentals/200_3_Pricing_Models/Code/Combined_EC2_RI_Rec.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Cost Opt\PublicWorkshops\aws-well-architected-labs\Cost\Cost_Fundamentals\200_3_Pricing_Models\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27525" windowHeight="12825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
   </bookViews>
   <sheets>
-    <sheet name="30Day Rec" sheetId="1" r:id="rId1"/>
-    <sheet name="7Day Rec" sheetId="2" r:id="rId2"/>
+    <sheet name="30_day_EC2_RI_Rec-1" sheetId="1" r:id="rId1"/>
+    <sheet name="7day Rec" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="65">
   <si>
     <t>Select all the lines below</t>
   </si>
@@ -212,13 +212,16 @@
   </si>
   <si>
     <t>7Day Recommendation</t>
+  </si>
+  <si>
+    <t>Fully Paid day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,14 +357,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,12 +560,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -714,16 +721,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1045,79 +1060,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="71.25" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="6">
         <v>11</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>8</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>10.84444444</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>98.585858590000001</v>
       </c>
       <c r="F2" t="s">
@@ -1129,38 +1150,45 @@
       <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="str">
+      <c r="I2">
+        <v>15268</v>
+      </c>
+      <c r="J2">
+        <v>1268.74</v>
+      </c>
+      <c r="K2" t="str">
         <f>CONCATENATE(A2,F2,G2,H2)</f>
         <v>c4.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>7</v>
       </c>
-      <c r="K2" s="4">
-        <f>VLOOKUP(I2,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="M2" s="7">
+        <f>VLOOKUP(K2,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>1591.310667</v>
       </c>
-      <c r="M2">
-        <v>5.8790044679999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>(I2+J2*12)/(I2/12+J2+N2)</f>
+        <v>7.3790044675277837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6">
         <v>100</v>
       </c>
       <c r="F3" t="s">
@@ -1172,39 +1200,46 @@
       <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I3">
+        <v>13422</v>
+      </c>
+      <c r="J3">
+        <v>1118.3599999999999</v>
+      </c>
+      <c r="K3" t="str">
         <f>CONCATENATE(A3,F3,G3,H3)</f>
-        <v>m4.10xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="4">
-        <f>VLOOKUP(I3,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
+        <v>r4.8xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
       <c r="L3">
-        <v>1314</v>
-      </c>
-      <c r="M3">
-        <v>6.8741778580000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M3" s="7">
+        <f>VLOOKUP(K3,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1491.396</v>
+      </c>
+      <c r="O3">
+        <f>(I3+J3*12)/(I3/12+J3+N3)</f>
+        <v>7.1996987331342064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4">
-        <v>38</v>
-      </c>
-      <c r="C4">
-        <v>32</v>
-      </c>
-      <c r="D4" s="4">
-        <v>37.279166670000002</v>
-      </c>
-      <c r="E4" s="4">
-        <v>98.370321439999998</v>
+        <v>46</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>100</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -1215,39 +1250,46 @@
       <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="str">
+      <c r="I4">
+        <v>14016</v>
+      </c>
+      <c r="J4">
+        <v>1168</v>
+      </c>
+      <c r="K4" t="str">
         <f>CONCATENATE(A4,F4,G4,H4)</f>
-        <v>m3.mediumUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J4">
+        <v>m4.10xlargeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" s="7">
+        <f>VLOOKUP(K4,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>1314</v>
+      </c>
+      <c r="O4">
+        <f>(I4+J4*12)/(I4/12+J4+N4)</f>
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>38</v>
+      </c>
+      <c r="C5">
         <v>32</v>
       </c>
-      <c r="K4">
-        <f>VLOOKUP(I4,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>25</v>
-      </c>
-      <c r="L4">
-        <v>992.77937499999996</v>
-      </c>
-      <c r="M4">
-        <v>5.7928071880000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>100</v>
+      <c r="D5" s="6">
+        <v>37.279166670000002</v>
+      </c>
+      <c r="E5" s="6">
+        <v>98.370321439999998</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
@@ -1258,39 +1300,46 @@
       <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" t="str">
+      <c r="I5">
+        <v>8621</v>
+      </c>
+      <c r="J5">
+        <v>819.68658330000005</v>
+      </c>
+      <c r="K5" t="str">
         <f>CONCATENATE(A5,F5,G5,H5)</f>
-        <v>c4.4xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J5">
+        <v>m3.mediumUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L5">
+        <v>32</v>
+      </c>
+      <c r="M5" s="2">
+        <f>VLOOKUP(K5,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="N5">
+        <v>992.77937499999996</v>
+      </c>
+      <c r="O5">
+        <f>(I5+J5*12)/(I5/12+J5+N5)</f>
+        <v>7.29280718810225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6">
         <v>3</v>
       </c>
-      <c r="K5" s="4">
-        <f>VLOOKUP(I5,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="C6" s="6">
         <v>3</v>
       </c>
-      <c r="L5">
-        <v>893.5</v>
-      </c>
-      <c r="M5">
-        <v>5.8014487419999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>120</v>
-      </c>
-      <c r="C6">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>46.429166670000001</v>
-      </c>
-      <c r="E6">
-        <v>77.863426090000004</v>
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6">
+        <v>100</v>
       </c>
       <c r="F6" t="s">
         <v>27</v>
@@ -1301,25 +1350,32 @@
       <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" t="str">
+      <c r="I6">
+        <v>8331</v>
+      </c>
+      <c r="J6">
+        <v>694.23</v>
+      </c>
+      <c r="K6" t="str">
         <f>CONCATENATE(A6,F6,G6,H6)</f>
-        <v>m4.largeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
-      </c>
-      <c r="K6">
-        <f>VLOOKUP(I6,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
+        <v>c4.4xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
       <c r="L6">
-        <v>756.31666670000004</v>
-      </c>
-      <c r="M6">
-        <v>6.2869539909999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M6" s="7">
+        <f>VLOOKUP(K6,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>893.5</v>
+      </c>
+      <c r="O6">
+        <f>(I6+J6*12)/(I6/12+J6+N6)</f>
+        <v>7.3014487418820506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1332,7 +1388,7 @@
       <c r="D7">
         <v>52.58888889</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="6">
         <v>96.222137329999995</v>
       </c>
       <c r="F7" t="s">
@@ -1344,25 +1400,32 @@
       <c r="H7" t="s">
         <v>29</v>
       </c>
-      <c r="I7" t="str">
+      <c r="I7">
+        <v>8200</v>
+      </c>
+      <c r="J7">
+        <v>809.67625559999999</v>
+      </c>
+      <c r="K7" t="str">
         <f>CONCATENATE(A7,F7,G7,H7)</f>
         <v>t2.mediumUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>48</v>
       </c>
-      <c r="K7" s="4">
-        <f>VLOOKUP(I7,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="M7" s="7">
+        <f>VLOOKUP(K7,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>50</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>748.95992220000005</v>
       </c>
-      <c r="M7">
-        <v>6.7929418750000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <f>(I7+J7*12)/(I7/12+J7+N7)</f>
+        <v>7.99123938939886</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1375,7 +1438,7 @@
       <c r="D8">
         <v>7.4722222220000001</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>94.526618229999997</v>
       </c>
       <c r="F8" t="s">
@@ -1387,38 +1450,45 @@
       <c r="H8" t="s">
         <v>29</v>
       </c>
-      <c r="I8" t="str">
+      <c r="I8">
+        <v>6524</v>
+      </c>
+      <c r="J8">
+        <v>751.20650000000001</v>
+      </c>
+      <c r="K8" t="str">
         <f>CONCATENATE(A8,F8,G8,H8)</f>
         <v>m3.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>7</v>
       </c>
-      <c r="K8" s="4">
-        <f>VLOOKUP(I8,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="M8" s="7">
+        <f>VLOOKUP(K8,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>734.2835</v>
       </c>
-      <c r="M8">
-        <v>6.1576038979999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <f>(I8+J8*12)/(I8/12+J8+N8)</f>
+        <v>7.6576038978426171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="6">
         <v>13</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="6">
         <v>11</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="6">
         <v>11.27638889</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="6">
         <v>98.640571129999998</v>
       </c>
       <c r="F9" t="s">
@@ -1430,38 +1500,45 @@
       <c r="H9" t="s">
         <v>29</v>
       </c>
-      <c r="I9" t="str">
+      <c r="I9">
+        <v>7711</v>
+      </c>
+      <c r="J9">
+        <v>692.84097220000001</v>
+      </c>
+      <c r="K9" t="str">
         <f>CONCATENATE(A9,F9,G9,H9)</f>
         <v>m4.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>4</v>
       </c>
-      <c r="K9" s="4">
-        <f>VLOOKUP(I9,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="M9" s="7">
+        <f>VLOOKUP(K9,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>722.51666669999997</v>
       </c>
-      <c r="M9">
-        <v>5.5810958900000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f>(I9+J9*12)/(I9/12+J9+N9)</f>
+        <v>7.7869539907207033</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
+        <v>59</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
         <v>100</v>
       </c>
       <c r="F10" t="s">
@@ -1473,82 +1550,96 @@
       <c r="H10" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="str">
+      <c r="I10">
+        <v>4656</v>
+      </c>
+      <c r="J10">
+        <v>727.08</v>
+      </c>
+      <c r="K10" t="str">
         <f>CONCATENATE(A10,F10,G10,H10)</f>
+        <v>m3.2xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" s="7">
+        <f>VLOOKUP(K10,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>708.46</v>
+      </c>
+      <c r="O10">
+        <f>(I10+J10*12)/(I10/12+J10+N10)</f>
+        <v>7.3379031992717465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>100</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11">
+        <v>3474</v>
+      </c>
+      <c r="J11">
+        <v>624.88</v>
+      </c>
+      <c r="K11" t="str">
+        <f>CONCATENATE(A11,F11,G11,H11)</f>
         <v>c3.4xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="4">
-        <f>VLOOKUP(I10,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L10">
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
+        <f>VLOOKUP(K11,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N11">
         <v>477</v>
       </c>
-      <c r="M10">
-        <v>6.3763964270000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="O11">
+        <f>(I11+J11*12)/(I11/12+J11+N11)</f>
+        <v>7.8860986933835466</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="6">
         <v>3</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C12" s="6">
         <v>3</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D12" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="6">
         <v>100</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" t="str">
-        <f>CONCATENATE(A11,F11,G11,H11)</f>
-        <v>c3.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4">
-        <f>VLOOKUP(I11,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="L11">
-        <v>414.38</v>
-      </c>
-      <c r="M11">
-        <v>6.2077970840000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="4">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4">
-        <v>11.04861111</v>
-      </c>
-      <c r="E12" s="4">
-        <v>99.733365410000005</v>
       </c>
       <c r="F12" t="s">
         <v>27</v>
@@ -1559,39 +1650,46 @@
       <c r="H12" t="s">
         <v>29</v>
       </c>
-      <c r="I12" t="str">
+      <c r="I12">
+        <v>4278</v>
+      </c>
+      <c r="J12">
+        <v>387.63</v>
+      </c>
+      <c r="K12" t="str">
         <f>CONCATENATE(A12,F12,G12,H12)</f>
-        <v>t2.largeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J12">
-        <v>11</v>
-      </c>
-      <c r="K12">
-        <f>VLOOKUP(I12,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>8</v>
+        <v>c3.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
       <c r="L12">
-        <v>337.7135778</v>
-      </c>
-      <c r="M12">
-        <v>6.4912393890000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7">
+        <f>VLOOKUP(K12,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>414.38</v>
+      </c>
+      <c r="O12">
+        <f>(I12+J12*12)/(I12/12+J12+N12)</f>
+        <v>7.7077970841857208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="4">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4">
-        <v>4</v>
-      </c>
-      <c r="E13" s="4">
-        <v>100</v>
+        <v>52</v>
+      </c>
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6">
+        <v>11.04861111</v>
+      </c>
+      <c r="E13" s="6">
+        <v>99.733365410000005</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
@@ -1602,38 +1700,45 @@
       <c r="H13" t="s">
         <v>29</v>
       </c>
-      <c r="I13" t="str">
+      <c r="I13">
+        <v>3597</v>
+      </c>
+      <c r="J13">
+        <v>304.58519999999999</v>
+      </c>
+      <c r="K13" t="str">
         <f>CONCATENATE(A13,F13,G13,H13)</f>
-        <v>t2.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J13">
+        <v>t2.largeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13" s="2">
+        <f>VLOOKUP(K13,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="N13">
+        <v>337.7135778</v>
+      </c>
+      <c r="O13">
+        <f>(I13+J13*12)/(I13/12+J13+N13)</f>
+        <v>7.6981389614834024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="K13" s="4">
-        <f>VLOOKUP(I13,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="C14" s="6">
         <v>4</v>
       </c>
-      <c r="L13">
-        <v>245.36266670000001</v>
-      </c>
-      <c r="M13">
-        <v>6.3860986930000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="4">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4">
-        <v>6</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="D14" s="6">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6">
         <v>100</v>
       </c>
       <c r="F14" t="s">
@@ -1645,39 +1750,46 @@
       <c r="H14" t="s">
         <v>29</v>
       </c>
-      <c r="I14" t="str">
+      <c r="I14">
+        <v>2620</v>
+      </c>
+      <c r="J14">
+        <v>218.416</v>
+      </c>
+      <c r="K14" t="str">
         <f>CONCATENATE(A14,F14,G14,H14)</f>
-        <v>m5.largeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J14">
-        <v>6</v>
-      </c>
-      <c r="K14" s="4">
-        <f>VLOOKUP(I14,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>6</v>
+        <v>t2.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
       <c r="L14">
-        <v>176.9</v>
-      </c>
-      <c r="M14">
-        <v>5.699698733</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="M14" s="7">
+        <f>VLOOKUP(K14,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>245.36266670000001</v>
+      </c>
+      <c r="O14">
+        <f>(I14+J14*12)/(I14/12+J14+N14)</f>
+        <v>7.6834771998497091</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15">
-        <v>62</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>33.002777780000002</v>
-      </c>
-      <c r="E15">
-        <v>78.512397800000002</v>
+        <v>57</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>100</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
@@ -1688,82 +1800,96 @@
       <c r="H15" t="s">
         <v>29</v>
       </c>
-      <c r="I15" t="str">
+      <c r="I15">
+        <v>1736</v>
+      </c>
+      <c r="J15">
+        <v>312.44</v>
+      </c>
+      <c r="K15" t="str">
         <f>CONCATENATE(A15,F15,G15,H15)</f>
-        <v>t2.mediumUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-      <c r="K15" s="6">
-        <f>VLOOKUP(I15,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>15</v>
+        <v>c3.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
       </c>
       <c r="L15">
-        <v>139.42772780000001</v>
-      </c>
-      <c r="M15">
-        <v>6.9627754619999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M15" s="7">
+        <f>VLOOKUP(K15,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>239.31333330000001</v>
+      </c>
+      <c r="O15">
+        <f>(I15+J15*12)/(I15/12+J15+N15)</f>
+        <v>7.8763964278202039</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
+        <v>45</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
         <v>100</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H16" t="s">
         <v>29</v>
       </c>
-      <c r="I16" t="str">
+      <c r="I16">
+        <v>1164</v>
+      </c>
+      <c r="J16">
+        <v>181.04</v>
+      </c>
+      <c r="K16" t="str">
         <f>CONCATENATE(A16,F16,G16,H16)</f>
-        <v>t2.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16" s="4">
-        <f>VLOOKUP(I16,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
+        <v>m3.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
       </c>
       <c r="L16">
-        <v>122.7543333</v>
-      </c>
-      <c r="M16">
-        <v>6.1981389619999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7">
+        <f>VLOOKUP(K16,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>177.48</v>
+      </c>
+      <c r="O16">
+        <f>(I16+J16*12)/(I16/12+J16+N16)</f>
+        <v>7.324552160168599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17">
-        <v>44</v>
-      </c>
-      <c r="C17">
-        <v>31</v>
-      </c>
-      <c r="D17">
-        <v>36.866666670000001</v>
-      </c>
-      <c r="E17" s="4">
-        <v>92.969291249999998</v>
+        <v>34</v>
+      </c>
+      <c r="B17" s="6">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6">
+        <v>6</v>
+      </c>
+      <c r="D17" s="6">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6">
+        <v>100</v>
       </c>
       <c r="F17" t="s">
         <v>27</v>
@@ -1774,553 +1900,696 @@
       <c r="H17" t="s">
         <v>29</v>
       </c>
-      <c r="I17" t="str">
+      <c r="I17">
+        <v>2082</v>
+      </c>
+      <c r="J17">
+        <v>175.2</v>
+      </c>
+      <c r="K17" t="str">
         <f>CONCATENATE(A17,F17,G17,H17)</f>
-        <v>t2.microUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J17">
-        <v>31</v>
-      </c>
-      <c r="K17" s="6">
-        <f>VLOOKUP(I17,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>32</v>
+        <v>m5.largeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
       <c r="L17">
-        <v>121.38296389999999</v>
-      </c>
-      <c r="M17">
-        <v>5.5599905529999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="7">
+        <f>VLOOKUP(K17,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="N17">
+        <v>176.9</v>
+      </c>
+      <c r="O17">
+        <f>(I17+J17*12)/(I17/12+J17+N17)</f>
+        <v>7.9611872146118712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>100</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18">
+        <v>1310</v>
+      </c>
+      <c r="J18">
+        <v>109.13500000000001</v>
+      </c>
+      <c r="K18" t="str">
+        <f>CONCATENATE(A18,F18,G18,H18)</f>
+        <v>t2.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7">
+        <f>VLOOKUP(K18,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>122.7543333</v>
+      </c>
+      <c r="O18">
+        <f>(I18+J18*12)/(I18/12+J18+N18)</f>
+        <v>7.6809087078251963</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="4" customFormat="1">
+      <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="B19" s="4">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
         <v>100</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="F19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="3" t="str">
-        <f>CONCATENATE(A18,F18,G18,H18)</f>
+      <c r="H19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="4">
+        <v>712</v>
+      </c>
+      <c r="J19" s="4">
+        <v>64.239999999999995</v>
+      </c>
+      <c r="K19" s="4" t="str">
+        <f>CONCATENATE(A19,F19,G19,H19)</f>
         <v>c3.largeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
-      <c r="J18" s="3">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3">
-        <f>VLOOKUP(I18,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L18" s="3">
+      <c r="L19" s="4">
+        <v>2</v>
+      </c>
+      <c r="M19" s="5">
+        <f>VLOOKUP(K19,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N19" s="4">
         <v>69.146666670000002</v>
       </c>
-      <c r="M18" s="3">
-        <v>6.1944790369999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1.994444444</v>
-      </c>
-      <c r="E19" s="3">
-        <v>99.722222220000006</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="O19" s="4">
+        <f>(I19+J19*12)/(I19/12+J19+N19)</f>
+        <v>7.6944790368117042</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="4" customFormat="1">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>100</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" s="3" t="str">
-        <f>CONCATENATE(A19,F19,G19,H19)</f>
-        <v>m4.largeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J19" s="3">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3">
-        <f>VLOOKUP(I19,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L19" s="3">
-        <v>61.094444490000001</v>
-      </c>
-      <c r="M19" s="3">
-        <v>6.9645514559999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>100</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="3" t="str">
+      <c r="H20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="4">
+        <v>517</v>
+      </c>
+      <c r="J20" s="4">
+        <v>43.07</v>
+      </c>
+      <c r="K20" s="4" t="str">
         <f>CONCATENATE(A20,F20,G20,H20)</f>
         <v>m4.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="K20" s="3">
-        <f>VLOOKUP(I20,'7Day Rec'!T$4:U$48,2,FALSE)</f>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="M20" s="5">
+        <f>VLOOKUP(K20,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="L20" s="3">
+      <c r="N20" s="4">
         <v>59.846666669999998</v>
       </c>
-      <c r="M20" s="3">
-        <v>6.4611872149999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="O20" s="4">
+        <f>(I20+J20*12)/(I20/12+J20+N20)</f>
+        <v>7.0810958902492915</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="4" customFormat="1">
+      <c r="A21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>100</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="4">
+        <v>120</v>
+      </c>
+      <c r="J21" s="4">
+        <v>9.9280000000000008</v>
+      </c>
+      <c r="K21" s="4" t="str">
+        <f>CONCATENATE(A21,F21,G21,H21)</f>
+        <v>t2.smallUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2</v>
+      </c>
+      <c r="M21" s="5">
+        <f>VLOOKUP(K21,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N21" s="4">
+        <v>13.651999999999999</v>
+      </c>
+      <c r="O21" s="4">
+        <f>(I21+J21*12)/(I21/12+J21+N21)</f>
+        <v>7.1213817748659931</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="4" customFormat="1">
+      <c r="A22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>100</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="4">
+        <v>30</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2.4820000000000002</v>
+      </c>
+      <c r="K22" s="4" t="str">
+        <f>CONCATENATE(A22,F22,G22,H22)</f>
+        <v>t2.microUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5">
+        <f>VLOOKUP(K22,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="B21" s="3">
-        <v>4</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2.0077399379999998</v>
-      </c>
-      <c r="E21" s="3">
-        <v>89.673607180000005</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="N22" s="4">
+        <v>3.4860000000000002</v>
+      </c>
+      <c r="O22" s="4">
+        <f>(I22+J22*12)/(I22/12+J22+N22)</f>
+        <v>7.0599905526688715</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" s="3" customFormat="1" ht="62.25" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>55</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>29.866666670000001</v>
+      </c>
+      <c r="E25">
+        <v>85.073765530000003</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25">
+        <v>65596</v>
+      </c>
+      <c r="J25">
+        <v>11949.67619</v>
+      </c>
+      <c r="K25" t="str">
+        <f>CONCATENATE(A25,F25,G25,H25)</f>
+        <v>c3.4xlargeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L25">
+        <v>22</v>
+      </c>
+      <c r="M25" s="2">
+        <f>VLOOKUP(K25,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="N25">
+        <v>5651.2118060000003</v>
+      </c>
+      <c r="O25">
+        <f>(I25+J25*12)/(I25/12+J25+N25)</f>
+        <v>9.0601339145359514</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>15.693055559999999</v>
+      </c>
+      <c r="E26">
+        <v>91.723581949999996</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26">
+        <v>21030</v>
+      </c>
+      <c r="J26">
+        <v>2244.75</v>
+      </c>
+      <c r="K26" t="str">
+        <f>CONCATENATE(A26,F26,G26,H26)</f>
+        <v>m4.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L26">
+        <v>15</v>
+      </c>
+      <c r="M26" s="2">
+        <f>VLOOKUP(K26,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="N26">
+        <v>1730.7152779999999</v>
+      </c>
+      <c r="O26">
+        <f>(I26+J26*12)/(I26/12+J26+N26)</f>
+        <v>8.3741778575774397</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>33.668055559999999</v>
+      </c>
+      <c r="E27">
+        <v>76.867976200000001</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27">
+        <v>13148</v>
+      </c>
+      <c r="J27">
+        <v>3956.0616249999998</v>
+      </c>
+      <c r="K27" t="str">
+        <f>CONCATENATE(A27,F27,G27,H27)</f>
+        <v>c4.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L27">
+        <v>18</v>
+      </c>
+      <c r="M27" s="2">
+        <f>VLOOKUP(K27,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="N27">
+        <v>1363.046333</v>
+      </c>
+      <c r="O27">
+        <f>(I27+J27*12)/(I27/12+J27+N27)</f>
+        <v>9.4501744873304965</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+      <c r="D28" s="8">
+        <v>24.581944440000001</v>
+      </c>
+      <c r="E28">
+        <v>84.765325669999996</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28">
+        <v>13514</v>
+      </c>
+      <c r="J28">
+        <v>1249.03</v>
+      </c>
+      <c r="K28" t="str">
+        <f>CONCATENATE(A28,F28,G28,H28)</f>
+        <v>m3.largeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L28">
+        <v>25</v>
+      </c>
+      <c r="M28" s="2">
+        <f>VLOOKUP(K28,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="N28">
+        <v>962.53975000000003</v>
+      </c>
+      <c r="O28">
+        <f>(I28+J28*12)/(I28/12+J28+N28)</f>
+        <v>8.5394280559951348</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>120</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29">
+        <v>46.429166670000001</v>
+      </c>
+      <c r="E29">
+        <v>77.863426090000004</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29">
+        <v>8050</v>
+      </c>
+      <c r="J29">
+        <v>2809.5114579999999</v>
+      </c>
+      <c r="K29" t="str">
+        <f>CONCATENATE(A29,F29,G29,H29)</f>
+        <v>m4.largeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29" s="2">
+        <f>VLOOKUP(K29,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N29">
+        <v>756.31666670000004</v>
+      </c>
+      <c r="O29">
+        <f>(I29+J29*12)/(I29/12+J29+N29)</f>
+        <v>9.8577943764680676</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <v>100</v>
+      </c>
+      <c r="F30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="3" t="str">
-        <f>CONCATENATE(A21,F21,G21,H21)</f>
-        <v>c5.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J21" s="3">
-        <v>2</v>
-      </c>
-      <c r="K21" s="3">
-        <f>VLOOKUP(I21,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L21" s="3">
-        <v>32.78538889</v>
-      </c>
-      <c r="M21" s="3">
-        <v>5.8379031990000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>100</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="H30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30">
+        <v>5049</v>
+      </c>
+      <c r="J30">
+        <v>227.03</v>
+      </c>
+      <c r="K30" t="str">
+        <f>CONCATENATE(A30,F30,G30,H30)</f>
+        <v>r3.2xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7">
+        <f>VLOOKUP(K30,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>264.72000000000003</v>
+      </c>
+      <c r="O30">
+        <f>(I30+J30*12)/(I30/12+J30+N30)</f>
+        <v>8.5187506849315078</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2.0847222219999999</v>
+      </c>
+      <c r="E31">
+        <v>98.734327640000004</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="3" t="str">
-        <f>CONCATENATE(A22,F22,G22,H22)</f>
-        <v>t2.mediumUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J22" s="3">
-        <v>1</v>
-      </c>
-      <c r="K22" s="3">
-        <f>VLOOKUP(I22,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>15</v>
-      </c>
-      <c r="L22" s="3">
-        <v>13.85766667</v>
-      </c>
-      <c r="M22" s="3">
-        <v>6.9501944870000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2</v>
-      </c>
-      <c r="C23" s="3">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3">
-        <v>100</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="3" t="str">
-        <f>CONCATENATE(A23,F23,G23,H23)</f>
-        <v>t2.smallUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J23" s="3">
-        <v>2</v>
-      </c>
-      <c r="K23" s="3">
-        <f>VLOOKUP(I23,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L23" s="3">
-        <v>13.651999999999999</v>
-      </c>
-      <c r="M23" s="3">
-        <v>6.1834771999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3">
-        <v>100</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="3" t="str">
-        <f>CONCATENATE(A24,F24,G24,H24)</f>
-        <v>t1.microUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J24" s="3">
-        <v>1</v>
-      </c>
-      <c r="K24" s="3">
-        <f>VLOOKUP(I24,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L24" s="3">
-        <v>3.5933333329999999</v>
-      </c>
-      <c r="M24" s="3">
-        <v>6.1809087070000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="H31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31">
+        <v>2966</v>
+      </c>
+      <c r="J31">
+        <v>274.2620139</v>
+      </c>
+      <c r="K31" t="str">
+        <f>CONCATENATE(A31,F31,G31,H31)</f>
+        <v>c4.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31" s="2">
+        <f>VLOOKUP(K31,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <v>155.7933333</v>
+      </c>
+      <c r="O31">
+        <f>(I31+J31*12)/(I31/12+J31+N31)</f>
+        <v>9.2394281914644374</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>100</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="3" t="str">
-        <f>CONCATENATE(A25,F25,G25,H25)</f>
-        <v>t2.microUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
-      <c r="K25" s="3">
-        <f>VLOOKUP(I25,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>32</v>
-      </c>
-      <c r="L25" s="3">
-        <v>3.4860000000000002</v>
-      </c>
-      <c r="M25" s="3">
-        <v>5.6213817749999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="3">
-        <v>6</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>2.5372460499999998</v>
-      </c>
-      <c r="E26" s="3">
-        <v>61.296936909999999</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="3" t="str">
-        <f>CONCATENATE(A26,F26,G26,H26)</f>
-        <v>m3.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J26" s="3">
-        <v>1</v>
-      </c>
-      <c r="K26" s="3">
-        <f>VLOOKUP(I26,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L26" s="3">
-        <v>0.86566666699999995</v>
-      </c>
-      <c r="M26" s="3">
-        <v>5.8245521599999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30">
-        <v>55</v>
-      </c>
-      <c r="C30">
-        <v>19</v>
-      </c>
-      <c r="D30">
-        <v>29.866666670000001</v>
-      </c>
-      <c r="E30">
-        <v>85.073765530000003</v>
-      </c>
-      <c r="F30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" t="str">
-        <f>CONCATENATE(A30,F30,G30,H30)</f>
-        <v>c3.4xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J30">
-        <v>22</v>
-      </c>
-      <c r="K30" s="5">
-        <f>VLOOKUP(I30,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>23</v>
-      </c>
-      <c r="L30">
-        <v>5651.2118060000003</v>
-      </c>
-      <c r="M30">
-        <v>7.5601339149999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31">
-        <v>24</v>
-      </c>
-      <c r="C31">
-        <v>12</v>
-      </c>
-      <c r="D31">
-        <v>15.693055559999999</v>
-      </c>
-      <c r="E31" s="4">
-        <v>91.723581949999996</v>
-      </c>
-      <c r="F31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G31" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" t="s">
-        <v>29</v>
-      </c>
-      <c r="I31" t="str">
-        <f>CONCATENATE(A31,F31,G31,H31)</f>
-        <v>m4.2xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J31">
-        <v>15</v>
-      </c>
-      <c r="K31" s="4">
-        <f>VLOOKUP(I31,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>15</v>
-      </c>
-      <c r="L31">
-        <v>1730.7152779999999</v>
-      </c>
-      <c r="M31">
-        <v>8.3577943769999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="4">
-        <v>2</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
-      </c>
-      <c r="D32" s="4">
-        <v>2</v>
-      </c>
-      <c r="E32" s="4">
-        <v>100</v>
+      <c r="B32">
+        <v>44</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>36.866666670000001</v>
+      </c>
+      <c r="E32">
+        <v>92.969291249999998</v>
       </c>
       <c r="F32" t="s">
         <v>27</v>
@@ -2331,760 +2600,837 @@
       <c r="H32" t="s">
         <v>29</v>
       </c>
-      <c r="I32" t="str">
+      <c r="I32">
+        <v>1312</v>
+      </c>
+      <c r="J32">
+        <v>162.20863610000001</v>
+      </c>
+      <c r="K32" t="str">
         <f>CONCATENATE(A32,F32,G32,H32)</f>
-        <v>r4.8xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J32">
-        <v>2</v>
-      </c>
-      <c r="K32" s="4">
-        <f>VLOOKUP(I32,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
+        <v>t2.microUS East (N. Virginia)Linux/UNIXShared</v>
       </c>
       <c r="L32">
-        <v>1491.396</v>
-      </c>
-      <c r="M32">
-        <v>7.5465753419999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M32" s="2">
+        <f>VLOOKUP(K32,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="N32">
+        <v>121.38296389999999</v>
+      </c>
+      <c r="O32">
+        <f>(I32+J32*12)/(I32/12+J32+N32)</f>
+        <v>8.2929418745633168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>4.0069444440000002</v>
+      </c>
+      <c r="E33">
+        <v>99.95923449</v>
+      </c>
+      <c r="F33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33">
+        <v>3000</v>
+      </c>
+      <c r="J33">
+        <v>252.1947222</v>
+      </c>
+      <c r="K33" t="str">
+        <f>CONCATENATE(A33,F33,G33,H33)</f>
+        <v>m5.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33" s="2">
+        <f>VLOOKUP(K33,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>117.92</v>
+      </c>
+      <c r="O33">
+        <f>(I33+J33*12)/(I33/12+J33+N33)</f>
+        <v>9.7180996526258578</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="4" customFormat="1">
+      <c r="A34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="4">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1.994444444</v>
+      </c>
+      <c r="E34" s="4">
+        <v>99.722222220000006</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1014</v>
+      </c>
+      <c r="J34" s="4">
+        <v>43.07</v>
+      </c>
+      <c r="K34" s="4" t="str">
+        <f>CONCATENATE(A34,F34,G34,H34)</f>
+        <v>m4.largeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L34" s="4">
+        <v>2</v>
+      </c>
+      <c r="M34" s="5">
+        <f>VLOOKUP(K34,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N34" s="4">
+        <v>61.094444490000001</v>
+      </c>
+      <c r="O34" s="4">
+        <f>(I34+J34*12)/(I34/12+J34+N34)</f>
+        <v>8.1140885032057071</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="4" customFormat="1">
+      <c r="A35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="4">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>2.286103394</v>
+      </c>
+      <c r="E35" s="4">
+        <v>99.861111109999996</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="4">
+        <v>876</v>
+      </c>
+      <c r="J35" s="4">
+        <v>37.96</v>
+      </c>
+      <c r="K35" s="4" t="str">
+        <f>CONCATENATE(A35,F35,G35,H35)</f>
+        <v>c5.largeUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2</v>
+      </c>
+      <c r="M35" s="5">
+        <f>VLOOKUP(K35,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N35" s="4">
+        <v>50.927638889999997</v>
+      </c>
+      <c r="O35" s="4">
+        <f>(I35+J35*12)/(I35/12+J35+N35)</f>
+        <v>8.2249639881692627</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="4" customFormat="1">
+      <c r="A36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="4">
+        <v>55</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>36.016530879999998</v>
+      </c>
+      <c r="E36" s="4">
+        <v>86.304089489999996</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I36" s="4">
+        <v>899</v>
+      </c>
+      <c r="J36" s="4">
+        <v>38.470999999999997</v>
+      </c>
+      <c r="K36" s="4" t="str">
+        <f>CONCATENATE(A36,F36,G36,H36)</f>
+        <v>t2.nanoUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L36" s="4">
+        <v>28</v>
+      </c>
+      <c r="M36" s="5">
+        <f>VLOOKUP(K36,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="N36" s="4">
+        <v>38.36090257</v>
+      </c>
+      <c r="O36" s="4">
+        <f>(I36+J36*12)/(I36/12+J36+N36)</f>
+        <v>8.9664898116958902</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="4" customFormat="1">
+      <c r="A37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="4">
+        <v>9</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1.168302945</v>
+      </c>
+      <c r="E37" s="4">
+        <v>95.152513920000004</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="4">
+        <v>748</v>
+      </c>
+      <c r="J37" s="4">
+        <v>89.79</v>
+      </c>
+      <c r="K37" s="4" t="str">
+        <f>CONCATENATE(A37,F37,G37,H37)</f>
+        <v>c4.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1</v>
+      </c>
+      <c r="M37" s="5">
+        <f>VLOOKUP(K37,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N37" s="4">
+        <v>35.371083329999998</v>
+      </c>
+      <c r="O37" s="4">
+        <f>(I37+J37*12)/(I37/12+J37+N37)</f>
+        <v>9.7361832554078038</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="4" customFormat="1">
+      <c r="A38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4">
+        <v>100</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I38" s="4">
+        <v>199</v>
+      </c>
+      <c r="J38" s="4">
+        <v>16.571000000000002</v>
+      </c>
+      <c r="K38" s="4" t="str">
+        <f>CONCATENATE(A38,F38,G38,H38)</f>
+        <v>t2.mediumUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1</v>
+      </c>
+      <c r="M38" s="5">
+        <f>VLOOKUP(K38,'7day Rec'!T$4:U$48,2,FALSE)</f>
         <v>15</v>
       </c>
-      <c r="D33">
-        <v>33.668055559999999</v>
-      </c>
-      <c r="E33">
-        <v>76.867976200000001</v>
-      </c>
-      <c r="F33" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="N38" s="4">
+        <v>13.85766667</v>
+      </c>
+      <c r="O38" s="4">
+        <f>(I38+J38*12)/(I38/12+J38+N38)</f>
+        <v>8.4627754609842327</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="4" customFormat="1">
+      <c r="A39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4">
+        <v>100</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H33" t="s">
-        <v>29</v>
-      </c>
-      <c r="I33" t="str">
-        <f>CONCATENATE(A33,F33,G33,H33)</f>
-        <v>c4.xlargeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J33">
-        <v>18</v>
-      </c>
-      <c r="K33" s="5">
-        <f>VLOOKUP(I33,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>19</v>
-      </c>
-      <c r="L33">
-        <v>1363.046333</v>
-      </c>
-      <c r="M33">
-        <v>7.950174487</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="H39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="4">
+        <v>62</v>
+      </c>
+      <c r="J39" s="4">
+        <v>5.84</v>
+      </c>
+      <c r="K39" s="4" t="str">
+        <f>CONCATENATE(A39,F39,G39,H39)</f>
+        <v>t1.microUS East (N. Virginia)Linux/UNIXShared</v>
+      </c>
+      <c r="L39" s="4">
+        <v>1</v>
+      </c>
+      <c r="M39" s="5">
+        <f>VLOOKUP(K39,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N39" s="4">
+        <v>3.5933333329999999</v>
+      </c>
+      <c r="O39" s="4">
+        <f>(I39+J39*12)/(I39/12+J39+N39)</f>
+        <v>9.0465753426722948</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="4" customFormat="1">
+      <c r="A40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="4">
+        <v>100</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="4">
+        <v>50</v>
+      </c>
+      <c r="J40" s="4">
+        <v>4.1609999999999996</v>
+      </c>
+      <c r="K40" s="4" t="str">
+        <f>CONCATENATE(A40,F40,G40,H40)</f>
+        <v>t2.microUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L40" s="4">
+        <v>1</v>
+      </c>
+      <c r="M40" s="5">
+        <f>VLOOKUP(K40,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N40" s="4">
+        <v>3.4983333330000002</v>
+      </c>
+      <c r="O40" s="4">
+        <f>(I40+J40*12)/(I40/12+J40+N40)</f>
+        <v>8.4501944869623475</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="4" customFormat="1">
+      <c r="A41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4">
+        <v>2</v>
+      </c>
+      <c r="D41" s="4">
+        <v>2</v>
+      </c>
+      <c r="E41" s="4">
+        <v>100</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" s="4">
+        <v>76</v>
+      </c>
+      <c r="J41" s="4">
+        <v>2.92</v>
+      </c>
+      <c r="K41" s="4" t="str">
+        <f>CONCATENATE(A41,F41,G41,H41)</f>
+        <v>t2.nanoEU (London)Linux/UNIXShared</v>
+      </c>
+      <c r="L41" s="4">
+        <v>2</v>
+      </c>
+      <c r="M41" s="5">
+        <f>VLOOKUP(K41,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N41" s="4">
+        <v>3.3026667299999999</v>
+      </c>
+      <c r="O41" s="4">
+        <f>(I41+J41*12)/(I41/12+J41+N41)</f>
+        <v>8.8435807135956139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="1:15" s="3" customFormat="1" ht="48" customHeight="1">
+      <c r="A43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>62</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>33.002777780000002</v>
+      </c>
+      <c r="E44">
+        <v>78.512397800000002</v>
+      </c>
+      <c r="F44" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44">
+        <v>3645</v>
+      </c>
+      <c r="J44">
+        <v>1397.4531939999999</v>
+      </c>
+      <c r="K44" t="str">
+        <f>CONCATENATE(A44,F44,G44,H44)</f>
+        <v>t2.mediumUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L44">
+        <v>12</v>
+      </c>
+      <c r="M44" s="2">
+        <f>VLOOKUP(K44,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="N44">
+        <v>139.42772780000001</v>
+      </c>
+      <c r="O44">
+        <f>(I44+J44*12)/(I44/12+J44+N44)</f>
+        <v>11.091000420679775</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="4" customFormat="1">
+      <c r="A45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="4">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1.888888889</v>
+      </c>
+      <c r="E45" s="4">
+        <v>89.042132010000003</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="4">
+        <v>1507</v>
+      </c>
+      <c r="J45" s="4">
+        <v>407.1777778</v>
+      </c>
+      <c r="K45" s="4" t="str">
+        <f>CONCATENATE(A45,F45,G45,H45)</f>
+        <v>m4.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+      <c r="M45" s="5">
+        <f>VLOOKUP(K45,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N45" s="4">
+        <v>65.676666670000003</v>
+      </c>
+      <c r="O45" s="4">
+        <f>(I45+J45*12)/(I45/12+J45+N45)</f>
+        <v>10.683037687004107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" s="4" customFormat="1">
+      <c r="A46" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="4">
+        <v>4</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
+        <v>2.0077399379999998</v>
+      </c>
+      <c r="E46" s="4">
+        <v>89.673607180000005</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="4">
+        <v>1396</v>
+      </c>
+      <c r="J46" s="4">
+        <v>117.82909720000001</v>
+      </c>
+      <c r="K46" s="4" t="str">
+        <f>CONCATENATE(A46,F46,G46,H46)</f>
+        <v>c5.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L46" s="4">
+        <v>2</v>
+      </c>
+      <c r="M46" s="5">
+        <f>VLOOKUP(K46,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N46" s="4">
+        <v>32.78538889</v>
+      </c>
+      <c r="O46" s="4">
+        <f>(I46+J46*12)/(I46/12+J46+N46)</f>
+        <v>10.526211348982416</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" s="4" customFormat="1">
+      <c r="A47" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.99722222199999999</v>
+      </c>
+      <c r="E47" s="4">
+        <v>99.722222220000006</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1307</v>
+      </c>
+      <c r="J47" s="4">
+        <v>54.75</v>
+      </c>
+      <c r="K47" s="4" t="str">
+        <f>CONCATENATE(A47,F47,G47,H47)</f>
+        <v>m5.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L47" s="4">
+        <v>1</v>
+      </c>
+      <c r="M47" s="5">
+        <f>VLOOKUP(K47,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N47" s="4">
+        <v>27.942111140000002</v>
+      </c>
+      <c r="O47" s="4">
+        <f>(I47+J47*12)/(I47/12+J47+N47)</f>
+        <v>10.250052333101756</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="4" customFormat="1">
+      <c r="A48" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="4">
+        <v>10</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <v>5.4323843419999998</v>
+      </c>
+      <c r="E48" s="4">
+        <v>73.079620759999997</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="4">
+        <v>900</v>
+      </c>
+      <c r="J48" s="4">
+        <v>360.29798890000001</v>
+      </c>
+      <c r="K48" s="4" t="str">
+        <f>CONCATENATE(A48,F48,G48,H48)</f>
+        <v>t2.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L48" s="4">
+        <v>2</v>
+      </c>
+      <c r="M48" s="5">
+        <f>VLOOKUP(K48,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="N48" s="4">
+        <v>12.916333330000001</v>
+      </c>
+      <c r="O48" s="4">
+        <f>(I48+J48*12)/(I48/12+J48+N48)</f>
+        <v>11.654192219497029</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="4" customFormat="1">
+      <c r="A49" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B34">
-        <v>29</v>
-      </c>
-      <c r="C34">
-        <v>16</v>
-      </c>
-      <c r="D34" s="5">
-        <v>24.581944440000001</v>
-      </c>
-      <c r="E34">
-        <v>84.765325669999996</v>
-      </c>
-      <c r="F34" t="s">
-        <v>27</v>
-      </c>
-      <c r="G34" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" t="s">
-        <v>29</v>
-      </c>
-      <c r="I34" t="str">
-        <f>CONCATENATE(A34,F34,G34,H34)</f>
-        <v>m3.largeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J34">
-        <v>25</v>
-      </c>
-      <c r="K34" s="4">
-        <f>VLOOKUP(I34,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>29</v>
-      </c>
-      <c r="L34">
-        <v>962.53975000000003</v>
-      </c>
-      <c r="M34">
-        <v>7.0394280560000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="4">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4">
-        <v>2</v>
-      </c>
-      <c r="D35" s="4">
-        <v>2</v>
-      </c>
-      <c r="E35" s="4">
-        <v>100</v>
-      </c>
-      <c r="F35" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="B49" s="4">
+        <v>6</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2.5372460499999998</v>
+      </c>
+      <c r="E49" s="4">
+        <v>61.296936909999999</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H35" t="s">
-        <v>29</v>
-      </c>
-      <c r="I35" t="str">
-        <f>CONCATENATE(A35,F35,G35,H35)</f>
-        <v>c3.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J35">
-        <v>2</v>
-      </c>
-      <c r="K35" s="4">
-        <f>VLOOKUP(I35,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L35">
-        <v>239.31333330000001</v>
-      </c>
-      <c r="M35">
-        <v>8.2361832550000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="4">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4">
-        <v>100</v>
-      </c>
-      <c r="F36" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" t="s">
-        <v>35</v>
-      </c>
-      <c r="H36" t="s">
-        <v>29</v>
-      </c>
-      <c r="I36" t="str">
-        <f>CONCATENATE(A36,F36,G36,H36)</f>
-        <v>m3.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36" s="4">
-        <f>VLOOKUP(I36,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>177.48</v>
-      </c>
-      <c r="M36">
-        <v>9.1830376870000006</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>2.0847222219999999</v>
-      </c>
-      <c r="E37" s="4">
-        <v>98.734327640000004</v>
-      </c>
-      <c r="F37" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" t="s">
-        <v>29</v>
-      </c>
-      <c r="I37" t="str">
-        <f>CONCATENATE(A37,F37,G37,H37)</f>
-        <v>c4.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J37">
-        <v>2</v>
-      </c>
-      <c r="K37" s="4">
-        <f>VLOOKUP(I37,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L37">
-        <v>155.7933333</v>
-      </c>
-      <c r="M37">
-        <v>9.0262113490000004</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38">
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
-        <v>4.0069444440000002</v>
-      </c>
-      <c r="E38" s="4">
-        <v>99.95923449</v>
-      </c>
-      <c r="F38" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" t="s">
-        <v>35</v>
-      </c>
-      <c r="H38" t="s">
-        <v>29</v>
-      </c>
-      <c r="I38" t="str">
-        <f>CONCATENATE(A38,F38,G38,H38)</f>
-        <v>m5.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J38">
-        <v>4</v>
-      </c>
-      <c r="K38">
-        <f>VLOOKUP(I38,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L38">
-        <v>117.92</v>
-      </c>
-      <c r="M38">
-        <v>7.0187506849999997</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="3">
-        <v>3</v>
-      </c>
-      <c r="C39" s="3">
-        <v>1</v>
-      </c>
-      <c r="D39" s="3">
-        <v>1.888888889</v>
-      </c>
-      <c r="E39" s="3">
-        <v>89.042132010000003</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I39" s="3" t="str">
-        <f>CONCATENATE(A39,F39,G39,H39)</f>
-        <v>m4.xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J39" s="3">
-        <v>1</v>
-      </c>
-      <c r="K39" s="3">
-        <f>VLOOKUP(I39,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L39" s="3">
-        <v>65.676666670000003</v>
-      </c>
-      <c r="M39" s="3">
-        <v>8.2180996529999994</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="3">
-        <v>3</v>
-      </c>
-      <c r="C40" s="3">
-        <v>0</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2.286103394</v>
-      </c>
-      <c r="E40" s="3">
-        <v>99.861111109999996</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I40" s="3" t="str">
-        <f>CONCATENATE(A40,F40,G40,H40)</f>
-        <v>c5.largeUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J40" s="3">
-        <v>2</v>
-      </c>
-      <c r="K40" s="3">
-        <f>VLOOKUP(I40,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L40" s="3">
-        <v>50.927638889999997</v>
-      </c>
-      <c r="M40" s="3">
-        <v>7.0686410869999996</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="3">
-        <v>55</v>
-      </c>
-      <c r="C41" s="3">
-        <v>0</v>
-      </c>
-      <c r="D41" s="3">
-        <v>36.016530879999998</v>
-      </c>
-      <c r="E41" s="3">
-        <v>86.304089489999996</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I41" s="3" t="str">
-        <f>CONCATENATE(A41,F41,G41,H41)</f>
-        <v>t2.nanoUS East (N. Virginia)Linux/UNIXShared</v>
-      </c>
-      <c r="J41" s="3">
-        <v>28</v>
-      </c>
-      <c r="K41" s="3">
-        <f>VLOOKUP(I41,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>31</v>
-      </c>
-      <c r="L41" s="3">
-        <v>38.36090257</v>
-      </c>
-      <c r="M41" s="3">
-        <v>7.9362578399999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="3">
-        <v>9</v>
-      </c>
-      <c r="C42" s="3">
-        <v>0</v>
-      </c>
-      <c r="D42" s="3">
-        <v>1.168302945</v>
-      </c>
-      <c r="E42" s="3">
-        <v>95.152513920000004</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" s="3" t="str">
-        <f>CONCATENATE(A42,F42,G42,H42)</f>
-        <v>c4.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J42" s="3">
-        <v>1</v>
-      </c>
-      <c r="K42" s="3">
-        <f>VLOOKUP(I42,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L42" s="3">
-        <v>35.371083329999998</v>
-      </c>
-      <c r="M42" s="3">
-        <v>7.739428191</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3">
-        <v>0</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0.99722222199999999</v>
-      </c>
-      <c r="E43" s="3">
-        <v>99.722222220000006</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I43" s="3" t="str">
-        <f>CONCATENATE(A43,F43,G43,H43)</f>
-        <v>m5.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J43" s="3">
-        <v>1</v>
-      </c>
-      <c r="K43" s="3">
-        <f>VLOOKUP(I43,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L43" s="3">
-        <v>27.942111140000002</v>
-      </c>
-      <c r="M43" s="3">
-        <v>9.5499902980000009</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="3">
-        <v>10</v>
-      </c>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3">
-        <v>5.4323843419999998</v>
-      </c>
-      <c r="E44" s="3">
-        <v>73.079620759999997</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I44" s="3" t="str">
-        <f>CONCATENATE(A44,F44,G44,H44)</f>
-        <v>t2.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J44" s="3">
-        <v>2</v>
-      </c>
-      <c r="K44" s="3">
-        <f>VLOOKUP(I44,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L44" s="3">
-        <v>12.916333330000001</v>
-      </c>
-      <c r="M44" s="3">
-        <v>9.5910004210000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3">
-        <v>1</v>
-      </c>
-      <c r="D45" s="3">
-        <v>1</v>
-      </c>
-      <c r="E45" s="3">
-        <v>100</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I45" s="3" t="str">
-        <f>CONCATENATE(A45,F45,G45,H45)</f>
-        <v>t2.microUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J45" s="3">
-        <v>1</v>
-      </c>
-      <c r="K45" s="3">
-        <f>VLOOKUP(I45,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L45" s="3">
-        <v>3.4983333330000002</v>
-      </c>
-      <c r="M45" s="3">
-        <v>8.4501944869999992</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="3">
-        <v>2</v>
-      </c>
-      <c r="C46" s="3">
-        <v>2</v>
-      </c>
-      <c r="D46" s="3">
-        <v>2</v>
-      </c>
-      <c r="E46" s="3">
-        <v>100</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I46" s="3" t="str">
-        <f>CONCATENATE(A46,F46,G46,H46)</f>
-        <v>t2.nanoEU (London)Linux/UNIXShared</v>
-      </c>
-      <c r="J46" s="3">
-        <v>2</v>
-      </c>
-      <c r="K46" s="3">
-        <f>VLOOKUP(I46,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L46" s="3">
-        <v>3.3026667299999999</v>
-      </c>
-      <c r="M46" s="3">
-        <v>7.887090079</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:13" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4">
-        <v>1</v>
-      </c>
-      <c r="E50" s="4">
-        <v>100</v>
-      </c>
-      <c r="F50" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" t="s">
-        <v>35</v>
-      </c>
-      <c r="H50" t="s">
-        <v>29</v>
-      </c>
-      <c r="I50" t="str">
-        <f>CONCATENATE(A50,F50,G50,H50)</f>
-        <v>r3.2xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-      <c r="K50" s="4">
-        <f>VLOOKUP(I50,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>264.72000000000003</v>
-      </c>
-      <c r="M50">
-        <v>10.154192220000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="4">
-        <v>2</v>
-      </c>
-      <c r="C51" s="4">
-        <v>2</v>
-      </c>
-      <c r="D51" s="4">
-        <v>2</v>
-      </c>
-      <c r="E51" s="4">
-        <v>100</v>
-      </c>
-      <c r="F51" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" t="s">
-        <v>35</v>
-      </c>
-      <c r="H51" t="s">
-        <v>29</v>
-      </c>
-      <c r="I51" t="str">
-        <f>CONCATENATE(A51,F51,G51,H51)</f>
-        <v>m3.2xlargeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
-      </c>
-      <c r="J51">
-        <v>2</v>
-      </c>
-      <c r="K51" s="4">
-        <f>VLOOKUP(I51,'7Day Rec'!T$4:U$48,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="L51">
-        <v>708.46</v>
-      </c>
-      <c r="M51">
-        <v>10.470784009999999</v>
+      <c r="H49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="4">
+        <v>585</v>
+      </c>
+      <c r="J49" s="4">
+        <v>305.94299999999998</v>
+      </c>
+      <c r="K49" s="4" t="str">
+        <f>CONCATENATE(A49,F49,G49,H49)</f>
+        <v>m3.largeUS East (N. Virginia)Windows (Amazon VPC)Shared</v>
+      </c>
+      <c r="L49" s="4">
+        <v>1</v>
+      </c>
+      <c r="M49" s="5">
+        <f>VLOOKUP(K49,'7day Rec'!T$4:U$48,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N49" s="4">
+        <v>0.86566666699999995</v>
+      </c>
+      <c r="O49" s="4">
+        <f>(I49+J49*12)/(I49/12+J49+N49)</f>
+        <v>11.970784005628728</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A30:X46">
-    <sortCondition descending="1" ref="L30:L46"/>
+  <sortState ref="A47:O52">
+    <sortCondition descending="1" ref="N47:N52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3092,13 +3438,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3106,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3114,7 +3460,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3185,7 +3531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3248,7 +3594,7 @@
         <v>6.9645514559999997</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3311,7 +3657,7 @@
         <v>7.0686410869999996</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -3374,7 +3720,7 @@
         <v>7.9362578399999997</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3437,7 +3783,7 @@
         <v>9.5499902980000009</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3500,7 +3846,7 @@
         <v>7.887090079</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3563,7 +3909,7 @@
         <v>6.2077970840000001</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3626,7 +3972,7 @@
         <v>7.5601339149999998</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3689,7 +4035,7 @@
         <v>6.1944790369999998</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3752,7 +4098,7 @@
         <v>5.8790044679999998</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -3815,7 +4161,7 @@
         <v>5.8014487419999998</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -3878,7 +4224,7 @@
         <v>7.950174487</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -3941,7 +4287,7 @@
         <v>7.0394280560000002</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -4004,7 +4350,7 @@
         <v>5.7928071880000003</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4067,7 +4413,7 @@
         <v>6.1576038979999996</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -4130,7 +4476,7 @@
         <v>6.8741778580000004</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4193,7 +4539,7 @@
         <v>8.3577943769999994</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -4256,7 +4602,7 @@
         <v>6.2869539909999999</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -4319,7 +4665,7 @@
         <v>5.5810958900000003</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -4382,7 +4728,7 @@
         <v>6.4611872149999998</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -4445,7 +4791,7 @@
         <v>5.699698733</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4508,7 +4854,7 @@
         <v>7.5465753419999997</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -4571,7 +4917,7 @@
         <v>6.1809087070000004</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -4634,7 +4980,7 @@
         <v>6.1981389619999998</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -4697,7 +5043,7 @@
         <v>6.4912393890000004</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -4760,7 +5106,7 @@
         <v>6.7929418750000004</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -4823,7 +5169,7 @@
         <v>5.5599905529999996</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -4886,7 +5232,7 @@
         <v>5.6213817749999997</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -4949,7 +5295,7 @@
         <v>6.1834771999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -5012,7 +5358,7 @@
         <v>6.3860986930000001</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -5075,7 +5421,7 @@
         <v>6.3763964270000004</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -5138,7 +5484,7 @@
         <v>8.2361832550000003</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -5201,7 +5547,7 @@
         <v>7.739428191</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -5264,7 +5610,7 @@
         <v>9.0262113490000004</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -5327,7 +5673,7 @@
         <v>5.8379031990000003</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -5390,7 +5736,7 @@
         <v>10.470784009999999</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -5453,7 +5799,7 @@
         <v>5.8245521599999996</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -5516,7 +5862,7 @@
         <v>9.1830376870000006</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -5579,7 +5925,7 @@
         <v>8.2180996529999994</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -5642,7 +5988,7 @@
         <v>7.0187506849999997</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -5705,7 +6051,7 @@
         <v>10.154192220000001</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -5768,7 +6114,7 @@
         <v>9.5910004210000004</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -5831,7 +6177,7 @@
         <v>6.9627754619999997</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -5894,7 +6240,7 @@
         <v>6.9501944870000001</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23">
       <c r="A48" t="s">
         <v>25</v>
       </c>

</xml_diff>